<commit_message>
append result columns (#2)
Co-authored-by: bojanth <b@profriday.com>
</commit_message>
<xml_diff>
--- a/examples/sample.xlsx
+++ b/examples/sample.xlsx
@@ -22,34 +22,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subcategory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">countryOfOrigin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grossMass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">netMass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weightUnit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customsTerritories</t>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subcategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country of origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customs territories</t>
   </si>
   <si>
     <t xml:space="preserve">Aldina shirt - Long sleeved blouses</t>
@@ -286,7 +286,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>